<commit_message>
Python Page Object Tests
</commit_message>
<xml_diff>
--- a/Computer Database Test Script.xlsx
+++ b/Computer Database Test Script.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decosta\Desktop\Backbase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Decosta\Desktop\Backbase\Backbase\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,6 +16,9 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
     <sheet name="Data" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Cases'!$A$5:$M$32</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="119">
   <si>
     <t>Test ID</t>
   </si>
@@ -719,6 +722,12 @@
   </si>
   <si>
     <t>Regression Tests</t>
+  </si>
+  <si>
+    <t>Test Case within Automation Suite</t>
+  </si>
+  <si>
+    <t>When user goes to main homepage, page should be loaded and return a 200 status code</t>
   </si>
 </sst>
 </file>
@@ -964,7 +973,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1027,6 +1036,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1556,10 +1568,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M32"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1576,9 +1589,10 @@
     <col min="10" max="11" width="22.28515625" customWidth="1"/>
     <col min="12" max="12" width="27.42578125" customWidth="1"/>
     <col min="13" max="13" width="19.5703125" customWidth="1"/>
+    <col min="14" max="14" width="80.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="27" t="s">
         <v>114</v>
       </c>
@@ -1586,19 +1600,19 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="28"/>
       <c r="B2" s="28"/>
       <c r="C2" s="28"/>
       <c r="D2" s="28"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="28"/>
       <c r="B3" s="28"/>
       <c r="C3" s="28"/>
       <c r="D3" s="28"/>
     </row>
-    <row r="5" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1636,8 +1650,11 @@
       <c r="M5" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="N5" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>1</v>
       </c>
@@ -1663,8 +1680,11 @@
       <c r="M6" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="N6" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2</v>
       </c>
@@ -1689,7 +1709,7 @@
       <c r="L7" s="9"/>
       <c r="M7" s="10"/>
     </row>
-    <row r="8" spans="1:13" ht="135" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>3</v>
       </c>
@@ -1719,8 +1739,9 @@
       <c r="M8" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="180" x14ac:dyDescent="0.25">
+      <c r="N8" s="9"/>
+    </row>
+    <row r="9" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>4</v>
       </c>
@@ -1748,8 +1769,9 @@
       <c r="M9" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="195" x14ac:dyDescent="0.25">
+      <c r="N9" s="9"/>
+    </row>
+    <row r="10" spans="1:14" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>5</v>
       </c>
@@ -1776,7 +1798,7 @@
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>6</v>
       </c>
@@ -1803,7 +1825,7 @@
       <c r="L11" s="9"/>
       <c r="M11" s="10"/>
     </row>
-    <row r="12" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>7</v>
       </c>
@@ -1830,7 +1852,7 @@
       <c r="L12" s="9"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>8</v>
       </c>
@@ -1857,7 +1879,7 @@
       <c r="L13" s="9"/>
       <c r="M13" s="10"/>
     </row>
-    <row r="14" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>9</v>
       </c>
@@ -1884,7 +1906,7 @@
       <c r="L14" s="9"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" ht="255" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>10</v>
       </c>
@@ -1912,8 +1934,9 @@
       <c r="M15" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="N15" s="9"/>
+    </row>
+    <row r="16" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>11</v>
       </c>
@@ -1942,7 +1965,7 @@
       <c r="L16" s="9"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>12</v>
       </c>
@@ -1972,8 +1995,9 @@
       <c r="M17" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="165" x14ac:dyDescent="0.25">
+      <c r="N17" s="9"/>
+    </row>
+    <row r="18" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>13</v>
       </c>
@@ -2003,8 +2027,9 @@
       <c r="M18" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="N18" s="9"/>
+    </row>
+    <row r="19" spans="1:14" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>14</v>
       </c>
@@ -2033,7 +2058,7 @@
       <c r="L19" s="9"/>
       <c r="M19" s="10"/>
     </row>
-    <row r="20" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="240" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>15</v>
       </c>
@@ -2060,7 +2085,7 @@
       <c r="L20" s="9"/>
       <c r="M20" s="10"/>
     </row>
-    <row r="21" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>16</v>
       </c>
@@ -2087,7 +2112,7 @@
       <c r="L21" s="9"/>
       <c r="M21" s="10"/>
     </row>
-    <row r="22" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>17</v>
       </c>
@@ -2113,7 +2138,7 @@
       <c r="L22" s="9"/>
       <c r="M22" s="10"/>
     </row>
-    <row r="23" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>18</v>
       </c>
@@ -2140,7 +2165,7 @@
       <c r="L23" s="9"/>
       <c r="M23" s="10"/>
     </row>
-    <row r="24" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>19</v>
       </c>
@@ -2167,7 +2192,7 @@
       <c r="L24" s="9"/>
       <c r="M24" s="10"/>
     </row>
-    <row r="25" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
         <v>20</v>
       </c>
@@ -2195,8 +2220,9 @@
       <c r="M25" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" ht="150" x14ac:dyDescent="0.25">
+      <c r="N25" s="9"/>
+    </row>
+    <row r="26" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>21</v>
       </c>
@@ -2224,8 +2250,9 @@
       <c r="M26" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+      <c r="N26" s="9"/>
+    </row>
+    <row r="27" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>22</v>
       </c>
@@ -2252,7 +2279,7 @@
       <c r="L27" s="9"/>
       <c r="M27" s="10"/>
     </row>
-    <row r="28" spans="1:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>23</v>
       </c>
@@ -2281,7 +2308,7 @@
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>
     </row>
-    <row r="29" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>24</v>
       </c>
@@ -2309,8 +2336,9 @@
       <c r="M29" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" ht="210" x14ac:dyDescent="0.25">
+      <c r="N29" s="9"/>
+    </row>
+    <row r="30" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>25</v>
       </c>
@@ -2340,8 +2368,9 @@
       <c r="M30" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" ht="240" x14ac:dyDescent="0.25">
+      <c r="N30" s="9"/>
+    </row>
+    <row r="31" spans="1:14" ht="240" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>26</v>
       </c>
@@ -2371,8 +2400,9 @@
       <c r="M31" s="10" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" ht="300" x14ac:dyDescent="0.25">
+      <c r="N31" s="9"/>
+    </row>
+    <row r="32" spans="1:14" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>27</v>
       </c>
@@ -2398,6 +2428,13 @@
       <c r="M32" s="10"/>
     </row>
   </sheetData>
+  <autoFilter ref="A5:M32">
+    <filterColumn colId="12">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="1">
     <mergeCell ref="A1:D3"/>
   </mergeCells>

</xml_diff>

<commit_message>
Added More Tests to finish assignment. Slight tweaks needed to 100 complete.
</commit_message>
<xml_diff>
--- a/Computer Database Test Script.xlsx
+++ b/Computer Database Test Script.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="128">
   <si>
     <t>Test ID</t>
   </si>
@@ -153,9 +153,6 @@
 4. Enter a discontinued date in the format yyyy-MM-dd (e.g. 2017-02-01)
 5. Choose a company from the Company drop down list (e.g. RCA)
 6. Click on 'Cancel'</t>
-  </si>
-  <si>
-    <t>The details of the computer within the text fields will not be commited to the database/table and the count will not increment.</t>
   </si>
   <si>
     <t>Read/Retrieve</t>
@@ -276,9 +273,6 @@
     <t>User attempts to add a computer entry without entering any details</t>
   </si>
   <si>
-    <t>The application will inform the user of any compulsory fields that have to be completed before a succesful submission.</t>
-  </si>
-  <si>
     <t>1. Navigate to http://computer-database.herokuapp.com/computers/new
 2. Click on Create this computer button
 3. Enter a computer name
@@ -290,31 +284,11 @@
     <t>User enters date (Introduced Date) on Add a computer screen in the wrong format</t>
   </si>
   <si>
-    <t>1. Navigate to http://computer-database.herokuapp.com/computers/new
-2. Enter a alphanumeric string in the Computer name field (e.g. A2-Computers)
-3. Enter an date in the Introduced Date field (e.g. 01 Feb 2017)
-4. Attempt to submit the form
-5. Enter a date in the Introduced Date field (e.g. 20-02-2017) 
-6. Attempt to submit the form
-7. Enter a date in the Introduced Date field (e.g 2017-02-30)
-8. Attempt to submit the form</t>
-  </si>
-  <si>
     <t xml:space="preserve">In each of the cases of invalid dates, the system will report/indicate to the user that the input is invalid
 </t>
   </si>
   <si>
     <t>User enters date (Discontinued Date) on Add a computer screen in the wrong format</t>
-  </si>
-  <si>
-    <t>1. Navigate to http://computer-database.herokuapp.com/computers/new
-2. Enter a alphanumeric string in the Computer name field (e.g. A2-Computers)
-3. Enter an date in the Discontinued Date field (e.g. 2017/2/17)
-4. Attempt to submit the form
-5. Enter a string in the Discontinued Date field (e.g. date) 
-6. Attempt to submit the form
-7. Enter a date in the Discontinued Date field (e.g 2017-02-30)
-8. Attempt to submit the form</t>
   </si>
   <si>
     <t>User ensures that the Form Data reflects the Added Computer Details</t>
@@ -494,12 +468,6 @@
     <t>User navigates to the Edit screen via direct URL</t>
   </si>
   <si>
-    <t>User attemps to navigate to the Edit screen for a computer that is not in the table.</t>
-  </si>
-  <si>
-    <t>User checks the Form Data for a computer entry that has been editted.</t>
-  </si>
-  <si>
     <t>1. Navigate to http://computer-database.herokuapp.com/computers
 2. Press F12 to open the console
 3. Click on the Network tab</t>
@@ -558,9 +526,6 @@
 4. When the main homepage loads and the success message is shown, look in the Name column in the Networks tab. Click on the Name that is a number
 5. In the Headers column, scroll down to the data under the Form Data section
 6. Check the data</t>
-  </si>
-  <si>
-    <t>The data within the Form Data of the page(within the Networks &gt; Headers) tab will reflect the changes made on the edit screen. Note that the entries in the company dropdown are numerial so the first entry will be 1.</t>
   </si>
   <si>
     <t>1. Navigate to http://computer-database.herokuapp.com/computers
@@ -728,6 +693,69 @@
   </si>
   <si>
     <t>When user goes to main homepage, page should be loaded and return a 200 status code</t>
+  </si>
+  <si>
+    <t>The user is able to add a computer entry via Homepage via direct link</t>
+  </si>
+  <si>
+    <t>The user searches for a computer using the filter text field</t>
+  </si>
+  <si>
+    <t>The user searches for a computer using the filter text field via direct link</t>
+  </si>
+  <si>
+    <t>The user edits a computer entry</t>
+  </si>
+  <si>
+    <t>The user edits a computer entry via a direct link</t>
+  </si>
+  <si>
+    <t>User checks the Form Data for a computer entry that has been edited.</t>
+  </si>
+  <si>
+    <t>The data within the Form Data of the page(within the Networks &gt; Headers) tab will reflect the changes made on the edit screen. Note that the entries in the company dropdown are numerical so the first entry will be 1.</t>
+  </si>
+  <si>
+    <t>User attempts to navigate to the Edit screen for a computer that is not in the table.</t>
+  </si>
+  <si>
+    <t>The details of the computer within the text fields will not be committed to the database/table and the count will not increment.</t>
+  </si>
+  <si>
+    <t>The application will inform the user of any compulsory fields that have to be completed before a successful submission.</t>
+  </si>
+  <si>
+    <t>1. Navigate to http://computer-database.herokuapp.com/computers/new
+2. Enter a alphanumeric string in the Computer name field (e.g. A2-Computers)
+3. Enter an date in the Introduced Date field (e.g. 01 Feb 2017)
+4. Attempt to submit the form
+5. Enter a date in the Introduced Date field (e.g. 20-02-2017) 
+6. Attempt to submit the form
+7. Enter a date in the Introduced Date field (e.g. 2017-02-30)
+8. Attempt to submit the form</t>
+  </si>
+  <si>
+    <t>1. Navigate to http://computer-database.herokuapp.com/computers/new
+2. Enter a alphanumeric string in the Computer name field (e.g. A2-Computers)
+3. Enter an date in the Discontinued Date field (e.g. 2017/2/17)
+4. Attempt to submit the form
+5. Enter a string in the Discontinued Date field (e.g. date) 
+6. Attempt to submit the form
+7. Enter a date in the Discontinued Date field (e.g. 2017-02-30)
+8. Attempt to submit the form</t>
+  </si>
+  <si>
+    <t>The user deletes the computer</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The user edits a computer entry via direct link for a computer not in the table
+</t>
+  </si>
+  <si>
+    <t>The user deletes the computer details via a direct link</t>
+  </si>
+  <si>
+    <t>The user inputs invalid computer names to attempt to break the website</t>
   </si>
 </sst>
 </file>
@@ -1020,6 +1048,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1036,9 +1067,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1412,105 +1440,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="20"/>
+      <c r="A1" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="21"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="23"/>
+      <c r="A2" s="22"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="23"/>
+      <c r="L2" s="23"/>
+      <c r="M2" s="23"/>
+      <c r="N2" s="24"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="22"/>
-      <c r="N3" s="23"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="24"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="21"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
-      <c r="M4" s="22"/>
-      <c r="N4" s="23"/>
+      <c r="A4" s="22"/>
+      <c r="B4" s="23"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="23"/>
+      <c r="I4" s="23"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24"/>
     </row>
     <row r="5" spans="1:14" ht="74.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+      <c r="K5" s="26"/>
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="27"/>
     </row>
     <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1551,7 +1579,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B18" s="10">
         <f>COUNTIF('Test Cases'!M$6:M$32,"Y")</f>
@@ -1571,8 +1599,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="G29" workbookViewId="0">
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1593,24 +1621,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
+      <c r="A1" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
+      <c r="A2" s="29"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
     </row>
     <row r="5" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -1650,8 +1678,8 @@
       <c r="M5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="N5" s="29" t="s">
-        <v>117</v>
+      <c r="N5" s="18" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -1678,10 +1706,10 @@
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
       <c r="M6" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -1717,7 +1745,7 @@
         <v>25</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>26</v>
@@ -1737,9 +1765,11 @@
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N8" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
@@ -1749,7 +1779,7 @@
         <v>25</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12" t="s">
@@ -1767,9 +1797,11 @@
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N9" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="195" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
@@ -1779,14 +1811,14 @@
         <v>25</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D10" s="11"/>
       <c r="E10" s="12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G10" s="11"/>
       <c r="H10" s="2"/>
@@ -1806,14 +1838,14 @@
         <v>25</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D11" s="11"/>
       <c r="E11" s="12" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>32</v>
+        <v>120</v>
       </c>
       <c r="G11" s="11"/>
       <c r="H11" s="2"/>
@@ -1833,14 +1865,14 @@
         <v>25</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>51</v>
+        <v>121</v>
       </c>
       <c r="G12" s="11"/>
       <c r="H12" s="2"/>
@@ -1860,14 +1892,14 @@
         <v>25</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="12" t="s">
-        <v>54</v>
+        <v>122</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="2"/>
@@ -1887,14 +1919,14 @@
         <v>25</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D14" s="10"/>
       <c r="E14" s="12" t="s">
-        <v>57</v>
+        <v>123</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="2"/>
@@ -1914,14 +1946,14 @@
         <v>25</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D15" s="10"/>
       <c r="E15" s="12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" s="2"/>
@@ -1932,28 +1964,30 @@
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N15" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N15" s="14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="16" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>11</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="12" t="s">
         <v>37</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>38</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" s="2"/>
@@ -1970,19 +2004,19 @@
         <v>12</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="12" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" s="13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" s="2"/>
@@ -1993,28 +2027,30 @@
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N17" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N17" s="14" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="18" spans="1:14" ht="165" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>13</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="F18" s="12" t="s">
         <v>40</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>41</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" s="2"/>
@@ -2025,28 +2061,30 @@
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="N18" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="N18" s="9"/>
     </row>
     <row r="19" spans="1:14" ht="210" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>14</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D19" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="12" t="s">
+      <c r="F19" s="12" t="s">
         <v>44</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>45</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" s="2"/>
@@ -2063,17 +2101,17 @@
         <v>15</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="12" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="2"/>
@@ -2090,17 +2128,17 @@
         <v>16</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F21" s="12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" s="2"/>
@@ -2117,16 +2155,16 @@
         <v>17</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" s="2"/>
@@ -2143,17 +2181,17 @@
         <v>18</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D23" s="11"/>
       <c r="E23" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G23" s="11"/>
       <c r="H23" s="2"/>
@@ -2170,17 +2208,17 @@
         <v>19</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D24" s="11"/>
       <c r="E24" s="12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="G24" s="11"/>
       <c r="H24" s="2"/>
@@ -2197,17 +2235,17 @@
         <v>20</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D25" s="11"/>
       <c r="E25" s="12" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="2"/>
@@ -2218,26 +2256,28 @@
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N25" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N25" s="14" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="26" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>21</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="F26" s="12" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G26" s="11"/>
       <c r="H26" s="2"/>
@@ -2248,26 +2288,28 @@
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N26" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N26" s="14" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>22</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="12" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="G27" s="11"/>
       <c r="H27" s="2"/>
@@ -2284,19 +2326,19 @@
         <v>23</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="G28" s="9"/>
       <c r="H28" s="2"/>
@@ -2313,17 +2355,17 @@
         <v>24</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>87</v>
+        <v>119</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="G29" s="9"/>
       <c r="H29" s="2"/>
@@ -2334,28 +2376,30 @@
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N29" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N29" s="15" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="30" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>25</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C30" s="14" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="F30" s="16" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="2"/>
@@ -2366,28 +2410,30 @@
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N30" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="240" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>26</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C31" s="14" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="F31" s="16" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="G31" s="9"/>
       <c r="H31" s="2"/>
@@ -2398,9 +2444,11 @@
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="N31" s="9"/>
+        <v>106</v>
+      </c>
+      <c r="N31" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="300" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
@@ -2409,13 +2457,13 @@
       <c r="B32" s="10"/>
       <c r="C32" s="9"/>
       <c r="D32" s="12" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="E32" s="16" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="F32" s="16" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="G32" s="9"/>
       <c r="H32" s="2"/>

</xml_diff>

<commit_message>
Add title to a test on main script tab
</commit_message>
<xml_diff>
--- a/Computer Database Test Script.xlsx
+++ b/Computer Database Test Script.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Overview" sheetId="3" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="1" r:id="rId2"/>
-    <sheet name="Data" sheetId="2" r:id="rId3"/>
+    <sheet name="Data" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Test Cases'!$A$5:$M$32</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="129">
   <si>
     <t>Test ID</t>
   </si>
@@ -756,6 +756,10 @@
   </si>
   <si>
     <t>The user inputs invalid computer names to attempt to break the website</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User deletes a computer entry via direct URL despite the method being POST 
+</t>
   </si>
 </sst>
 </file>
@@ -1430,7 +1434,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1596,11 +1600,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G29" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1712,7 +1715,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="10">
         <v>2</v>
       </c>
@@ -1736,6 +1739,7 @@
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
       <c r="M7" s="10"/>
+      <c r="N7" s="9"/>
     </row>
     <row r="8" spans="1:14" ht="135" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
@@ -1803,7 +1807,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="195" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" ht="195" x14ac:dyDescent="0.25">
       <c r="A10" s="10">
         <v>5</v>
       </c>
@@ -1829,8 +1833,9 @@
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:14" ht="90" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N10" s="9"/>
+    </row>
+    <row r="11" spans="1:14" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>6</v>
       </c>
@@ -1856,8 +1861,9 @@
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N11" s="9"/>
+    </row>
+    <row r="12" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>7</v>
       </c>
@@ -1883,8 +1889,9 @@
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:14" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N12" s="9"/>
+    </row>
+    <row r="13" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>8</v>
       </c>
@@ -1910,8 +1917,9 @@
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="10"/>
-    </row>
-    <row r="14" spans="1:14" ht="120" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N13" s="9"/>
+    </row>
+    <row r="14" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>9</v>
       </c>
@@ -1937,6 +1945,7 @@
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="10"/>
+      <c r="N14" s="9"/>
     </row>
     <row r="15" spans="1:14" ht="255" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
@@ -1970,7 +1979,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>11</v>
       </c>
@@ -1998,6 +2007,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="10"/>
+      <c r="N16" s="9"/>
     </row>
     <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
@@ -2067,7 +2077,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="210" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="210" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>14</v>
       </c>
@@ -2095,8 +2105,9 @@
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="10"/>
-    </row>
-    <row r="20" spans="1:14" ht="240" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N19" s="9"/>
+    </row>
+    <row r="20" spans="1:14" ht="240" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>15</v>
       </c>
@@ -2122,8 +2133,9 @@
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="10"/>
-    </row>
-    <row r="21" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="9"/>
+    </row>
+    <row r="21" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>16</v>
       </c>
@@ -2149,8 +2161,9 @@
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="10"/>
-    </row>
-    <row r="22" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N21" s="9"/>
+    </row>
+    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="10">
         <v>17</v>
       </c>
@@ -2175,8 +2188,9 @@
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="10"/>
-    </row>
-    <row r="23" spans="1:14" ht="45" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N22" s="9"/>
+    </row>
+    <row r="23" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="10">
         <v>18</v>
       </c>
@@ -2202,8 +2216,9 @@
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="10"/>
-    </row>
-    <row r="24" spans="1:14" ht="60" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="10">
         <v>19</v>
       </c>
@@ -2229,6 +2244,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="10"/>
+      <c r="N24" s="9"/>
     </row>
     <row r="25" spans="1:14" ht="150" x14ac:dyDescent="0.25">
       <c r="A25" s="10">
@@ -2294,7 +2310,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>22</v>
       </c>
@@ -2320,8 +2336,9 @@
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="10"/>
-    </row>
-    <row r="28" spans="1:14" ht="105" hidden="1" x14ac:dyDescent="0.25">
+      <c r="N27" s="9"/>
+    </row>
+    <row r="28" spans="1:14" ht="105" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>23</v>
       </c>
@@ -2349,6 +2366,7 @@
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>
+      <c r="N28" s="9"/>
     </row>
     <row r="29" spans="1:14" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
@@ -2450,12 +2468,16 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:14" ht="300" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" ht="300" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>27</v>
       </c>
-      <c r="B32" s="10"/>
-      <c r="C32" s="9"/>
+      <c r="B32" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>128</v>
+      </c>
       <c r="D32" s="12" t="s">
         <v>103</v>
       </c>
@@ -2474,15 +2496,10 @@
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="10"/>
+      <c r="N32" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A5:M32">
-    <filterColumn colId="12">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A5:M32"/>
   <mergeCells count="1">
     <mergeCell ref="A1:D3"/>
   </mergeCells>

</xml_diff>